<commit_message>
Property file and Csv Files
</commit_message>
<xml_diff>
--- a/Project_161/Testdata/InputData.xlsx
+++ b/Project_161/Testdata/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="7950" windowHeight="3495" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="7950" windowHeight="3495" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,6 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:C10"/>
 </workbook>
 </file>
 
@@ -1077,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:B30"/>
     </sheetView>
   </sheetViews>
@@ -1339,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:B23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1666,20 +1665,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H8" sqref="A7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">

</xml_diff>